<commit_message>
atualização e inserção de gráficos de gastos
alteração dos eixos gráficos de consultas.

modificação do gráfico despesas sjc.

adicionado graficos de despesas com medicamentos para sjc e caçapava.
</commit_message>
<xml_diff>
--- a/Dados/Dados de Medicamentos/São José dos Campos/med-sjc.xlsx
+++ b/Dados/Dados de Medicamentos/São José dos Campos/med-sjc.xlsx
@@ -1,34 +1,46 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gabri\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gabri\OneDrive\Área de Trabalho\fatec\API\Dados\Dados de Medicamentos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B241CDB1-FCBB-4B9A-904E-5F4B58EB71FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FBFAAD0-E3CB-4E0D-A02E-4B5082D9284C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2022" sheetId="1" r:id="rId1"/>
     <sheet name="2020" sheetId="2" r:id="rId2"/>
     <sheet name="2019" sheetId="3" r:id="rId3"/>
-    <sheet name="Planilha3" sheetId="4" r:id="rId4"/>
+    <sheet name="2021" sheetId="4" r:id="rId4"/>
+    <sheet name="Planilha1" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="128">
   <si>
     <t>Período</t>
   </si>
@@ -406,13 +418,23 @@
   </si>
   <si>
     <t>https://servicos.sjc.sp.gov.br/portal_da_transparencia/despesa_fornecedor.aspx</t>
+  </si>
+  <si>
+    <t>total gasto</t>
+  </si>
+  <si>
+    <t>ano</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="2">
+    <numFmt numFmtId="44" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="&quot;R$&quot;\ #,##0.00"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -422,6 +444,13 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -446,17 +475,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Moeda" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -470,6 +502,1022 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="pt-BR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Total gasto com medicamentos em São José dos Campos</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pt-BR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Planilha1!$B$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>total gasto</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-D02F-423D-82AB-CD7ECC6A382B}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000002-D02F-423D-82AB-CD7ECC6A382B}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="7030A0"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-D02F-423D-82AB-CD7ECC6A382B}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:cat>
+            <c:numRef>
+              <c:f>Planilha1!$A$3:$A$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>2019</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2020</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2021</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2022</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Planilha1!$B$3:$B$6</c:f>
+              <c:numCache>
+                <c:formatCode>"R$"\ #,##0.00</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>4353742.7300000004</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3873657.01</c:v>
+                </c:pt>
+                <c:pt idx="2" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
+                  <c:v>5070006.37</c:v>
+                </c:pt>
+                <c:pt idx="3" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)">
+                  <c:v>4593269.88</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-D02F-423D-82AB-CD7ECC6A382B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1448079183"/>
+        <c:axId val="1448080143"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1448079183"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1448080143"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1448080143"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pt-BR"/>
+                  <a:t>Valor gasto</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="pt-BR"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="&quot;R$&quot;\ #,##0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1448079183"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="pt-BR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>202659</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>95655</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>518808</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>42153</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Gráfico 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4FF960AC-6DB7-331F-D3E9-4F80167E1543}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -735,10 +1783,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N42"/>
+  <dimension ref="A1:H43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="M11" sqref="M11"/>
+    <sheetView topLeftCell="C18" workbookViewId="0">
+      <selection activeCell="F43" sqref="F43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -746,27 +1794,28 @@
     <col min="2" max="2" width="79.88671875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.77734375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17.77734375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>2022</v>
       </c>
@@ -779,11 +1828,11 @@
       <c r="D2" t="s">
         <v>6</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="3">
         <v>149.86000000000001</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2022</v>
       </c>
@@ -796,23 +1845,17 @@
       <c r="D3" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="2">
+      <c r="E3" s="3">
         <v>487501.01</v>
       </c>
       <c r="G3" t="s">
         <v>124</v>
       </c>
-      <c r="H3" s="4" t="s">
+      <c r="H3" t="s">
         <v>125</v>
       </c>
-      <c r="I3" s="4"/>
-      <c r="J3" s="4"/>
-      <c r="K3" s="4"/>
-      <c r="L3" s="4"/>
-      <c r="M3" s="4"/>
-      <c r="N3" s="4"/>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2022</v>
       </c>
@@ -825,11 +1868,11 @@
       <c r="D4" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="2">
+      <c r="E4" s="3">
         <v>42325</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>2022</v>
       </c>
@@ -842,11 +1885,11 @@
       <c r="D5" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="2">
+      <c r="E5" s="3">
         <v>30456.2</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>2022</v>
       </c>
@@ -859,11 +1902,11 @@
       <c r="D6" t="s">
         <v>14</v>
       </c>
-      <c r="E6" s="2">
+      <c r="E6" s="3">
         <v>13065.64</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>2022</v>
       </c>
@@ -876,11 +1919,11 @@
       <c r="D7" t="s">
         <v>16</v>
       </c>
-      <c r="E7" s="2">
+      <c r="E7" s="3">
         <v>442514.4</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>2022</v>
       </c>
@@ -893,11 +1936,11 @@
       <c r="D8" t="s">
         <v>18</v>
       </c>
-      <c r="E8" s="2">
+      <c r="E8" s="3">
         <v>48043.1</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>2022</v>
       </c>
@@ -910,11 +1953,11 @@
       <c r="D9" t="s">
         <v>20</v>
       </c>
-      <c r="E9" s="2">
+      <c r="E9" s="3">
         <v>88461.31</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>2022</v>
       </c>
@@ -927,11 +1970,11 @@
       <c r="D10" t="s">
         <v>21</v>
       </c>
-      <c r="E10" s="2">
+      <c r="E10" s="3">
         <v>715671.69</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>2022</v>
       </c>
@@ -944,11 +1987,11 @@
       <c r="D11" t="s">
         <v>23</v>
       </c>
-      <c r="E11" s="2">
+      <c r="E11" s="3">
         <v>134166.37</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>2022</v>
       </c>
@@ -961,11 +2004,11 @@
       <c r="D12" t="s">
         <v>25</v>
       </c>
-      <c r="E12" s="2">
+      <c r="E12" s="3">
         <v>6398</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>2022</v>
       </c>
@@ -978,11 +2021,11 @@
       <c r="D13" t="s">
         <v>27</v>
       </c>
-      <c r="E13" s="2">
+      <c r="E13" s="3">
         <v>9964.98</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>2022</v>
       </c>
@@ -995,11 +2038,11 @@
       <c r="D14" t="s">
         <v>29</v>
       </c>
-      <c r="E14" s="2">
+      <c r="E14" s="3">
         <v>93543.5</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>2022</v>
       </c>
@@ -1012,11 +2055,11 @@
       <c r="D15" t="s">
         <v>31</v>
       </c>
-      <c r="E15" s="2">
+      <c r="E15" s="3">
         <v>98280</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>2022</v>
       </c>
@@ -1029,7 +2072,7 @@
       <c r="D16" t="s">
         <v>33</v>
       </c>
-      <c r="E16" s="2">
+      <c r="E16" s="3">
         <v>7780</v>
       </c>
     </row>
@@ -1046,7 +2089,7 @@
       <c r="D17" t="s">
         <v>35</v>
       </c>
-      <c r="E17" s="2">
+      <c r="E17" s="3">
         <v>62376</v>
       </c>
     </row>
@@ -1063,7 +2106,7 @@
       <c r="D18" t="s">
         <v>37</v>
       </c>
-      <c r="E18" s="2">
+      <c r="E18" s="3">
         <v>3388</v>
       </c>
     </row>
@@ -1080,7 +2123,7 @@
       <c r="D19" t="s">
         <v>39</v>
       </c>
-      <c r="E19" s="2">
+      <c r="E19" s="3">
         <v>392393.51</v>
       </c>
     </row>
@@ -1097,7 +2140,7 @@
       <c r="D20" t="s">
         <v>41</v>
       </c>
-      <c r="E20" s="2">
+      <c r="E20" s="3">
         <v>10800</v>
       </c>
     </row>
@@ -1114,7 +2157,7 @@
       <c r="D21" t="s">
         <v>43</v>
       </c>
-      <c r="E21">
+      <c r="E21" s="3">
         <v>336</v>
       </c>
     </row>
@@ -1131,7 +2174,7 @@
       <c r="D22" t="s">
         <v>45</v>
       </c>
-      <c r="E22" s="2">
+      <c r="E22" s="3">
         <v>17982.2</v>
       </c>
     </row>
@@ -1148,7 +2191,7 @@
       <c r="D23" t="s">
         <v>47</v>
       </c>
-      <c r="E23" s="2">
+      <c r="E23" s="3">
         <v>11213.1</v>
       </c>
     </row>
@@ -1165,7 +2208,7 @@
       <c r="D24" t="s">
         <v>49</v>
       </c>
-      <c r="E24" s="2">
+      <c r="E24" s="3">
         <v>93460.79</v>
       </c>
     </row>
@@ -1182,7 +2225,7 @@
       <c r="D25" t="s">
         <v>51</v>
       </c>
-      <c r="E25" s="2">
+      <c r="E25" s="3">
         <v>51668.2</v>
       </c>
     </row>
@@ -1199,7 +2242,7 @@
       <c r="D26" t="s">
         <v>53</v>
       </c>
-      <c r="E26" s="2">
+      <c r="E26" s="3">
         <v>5874</v>
       </c>
     </row>
@@ -1216,7 +2259,7 @@
       <c r="D27" t="s">
         <v>55</v>
       </c>
-      <c r="E27" s="2">
+      <c r="E27" s="3">
         <v>15615.84</v>
       </c>
     </row>
@@ -1233,7 +2276,7 @@
       <c r="D28" t="s">
         <v>57</v>
       </c>
-      <c r="E28" s="2">
+      <c r="E28" s="3">
         <v>59777.18</v>
       </c>
     </row>
@@ -1250,7 +2293,7 @@
       <c r="D29" t="s">
         <v>59</v>
       </c>
-      <c r="E29" s="2">
+      <c r="E29" s="3">
         <v>5287.7</v>
       </c>
     </row>
@@ -1267,7 +2310,7 @@
       <c r="D30" t="s">
         <v>61</v>
       </c>
-      <c r="E30" s="2">
+      <c r="E30" s="3">
         <v>5130</v>
       </c>
     </row>
@@ -1284,7 +2327,7 @@
       <c r="D31" t="s">
         <v>63</v>
       </c>
-      <c r="E31" s="2">
+      <c r="E31" s="3">
         <v>111866</v>
       </c>
     </row>
@@ -1301,11 +2344,11 @@
       <c r="D32" t="s">
         <v>65</v>
       </c>
-      <c r="E32" s="2">
+      <c r="E32" s="3">
         <v>489409.3</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>2022</v>
       </c>
@@ -1318,11 +2361,11 @@
       <c r="D33" t="s">
         <v>67</v>
       </c>
-      <c r="E33" s="2">
+      <c r="E33" s="3">
         <v>113068.3</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>2022</v>
       </c>
@@ -1335,11 +2378,11 @@
       <c r="D34" t="s">
         <v>69</v>
       </c>
-      <c r="E34" s="2">
+      <c r="E34" s="3">
         <v>209020</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>2022</v>
       </c>
@@ -1352,11 +2395,11 @@
       <c r="D35" t="s">
         <v>71</v>
       </c>
-      <c r="E35" s="2">
+      <c r="E35" s="3">
         <v>236458.46</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>2022</v>
       </c>
@@ -1369,11 +2412,11 @@
       <c r="D36" t="s">
         <v>73</v>
       </c>
-      <c r="E36" s="2">
+      <c r="E36" s="3">
         <v>5104.4399999999996</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>2022</v>
       </c>
@@ -1386,11 +2429,11 @@
       <c r="D37" t="s">
         <v>75</v>
       </c>
-      <c r="E37">
+      <c r="E37" s="3">
         <v>747</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>2022</v>
       </c>
@@ -1403,11 +2446,11 @@
       <c r="D38" t="s">
         <v>77</v>
       </c>
-      <c r="E38" s="2">
+      <c r="E38" s="3">
         <v>12239.6</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>2022</v>
       </c>
@@ -1420,11 +2463,11 @@
       <c r="D39" t="s">
         <v>79</v>
       </c>
-      <c r="E39" s="2">
+      <c r="E39" s="3">
         <v>398445.89</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>2022</v>
       </c>
@@ -1437,11 +2480,11 @@
       <c r="D40" t="s">
         <v>81</v>
       </c>
-      <c r="E40" s="2">
+      <c r="E40" s="3">
         <v>1566.43</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>2022</v>
       </c>
@@ -1454,11 +2497,11 @@
       <c r="D41" t="s">
         <v>83</v>
       </c>
-      <c r="E41" s="2">
+      <c r="E41" s="3">
         <v>9600</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>2022</v>
       </c>
@@ -1471,8 +2514,17 @@
       <c r="D42" t="s">
         <v>85</v>
       </c>
-      <c r="E42" s="2">
+      <c r="E42" s="3">
         <v>52120.88</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E43" s="3">
+        <f>SUM(E2:E42)</f>
+        <v>4593269.88</v>
+      </c>
+      <c r="F43" s="5">
+        <v>4593269.88</v>
       </c>
     </row>
   </sheetData>
@@ -1483,10 +2535,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3065164-8D2E-4D2B-9ABD-DB354CC38A13}">
-  <dimension ref="A1:E25"/>
+  <dimension ref="A1:F26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:E1"/>
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1494,27 +2546,27 @@
     <col min="2" max="2" width="72.44140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.77734375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17.77734375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="14.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>2020</v>
       </c>
@@ -1527,11 +2579,12 @@
       <c r="D2" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="2">
+      <c r="E2" s="3">
         <v>281129.56</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F2" s="3"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2020</v>
       </c>
@@ -1544,11 +2597,12 @@
       <c r="D3" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="2">
+      <c r="E3" s="3">
         <v>4550</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F3" s="3"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2020</v>
       </c>
@@ -1561,11 +2615,12 @@
       <c r="D4" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="2">
+      <c r="E4" s="3">
         <v>10419.64</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F4" s="3"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>2020</v>
       </c>
@@ -1578,11 +2633,12 @@
       <c r="D5" t="s">
         <v>16</v>
       </c>
-      <c r="E5" s="2">
+      <c r="E5" s="3">
         <v>8955</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F5" s="3"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>2020</v>
       </c>
@@ -1595,11 +2651,12 @@
       <c r="D6" t="s">
         <v>20</v>
       </c>
-      <c r="E6" s="2">
+      <c r="E6" s="3">
         <v>66214.41</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F6" s="3"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>2020</v>
       </c>
@@ -1612,11 +2669,12 @@
       <c r="D7" t="s">
         <v>87</v>
       </c>
-      <c r="E7" s="2">
+      <c r="E7" s="3">
         <v>156965.6</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F7" s="3"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>2020</v>
       </c>
@@ -1629,11 +2687,12 @@
       <c r="D8" t="s">
         <v>27</v>
       </c>
-      <c r="E8" s="2">
+      <c r="E8" s="3">
         <v>18000</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F8" s="3"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>2020</v>
       </c>
@@ -1646,11 +2705,12 @@
       <c r="D9" t="s">
         <v>35</v>
       </c>
-      <c r="E9" s="2">
+      <c r="E9" s="3">
         <v>135568.12</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F9" s="3"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>2020</v>
       </c>
@@ -1663,11 +2723,12 @@
       <c r="D10" t="s">
         <v>89</v>
       </c>
-      <c r="E10" s="2">
+      <c r="E10" s="3">
         <v>16323.6</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F10" s="3"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>2020</v>
       </c>
@@ -1680,11 +2741,12 @@
       <c r="D11" t="s">
         <v>91</v>
       </c>
-      <c r="E11" s="2">
+      <c r="E11" s="3">
         <v>11968.4</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F11" s="3"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>2020</v>
       </c>
@@ -1697,11 +2759,12 @@
       <c r="D12" t="s">
         <v>41</v>
       </c>
-      <c r="E12" s="2">
+      <c r="E12" s="3">
         <v>46990</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F12" s="3"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>2020</v>
       </c>
@@ -1714,11 +2777,12 @@
       <c r="D13" t="s">
         <v>45</v>
       </c>
-      <c r="E13" s="2">
+      <c r="E13" s="3">
         <v>171564</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F13" s="3"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>2020</v>
       </c>
@@ -1731,11 +2795,12 @@
       <c r="D14" t="s">
         <v>93</v>
       </c>
-      <c r="E14" s="2">
+      <c r="E14" s="3">
         <v>33550</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F14" s="3"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>2020</v>
       </c>
@@ -1748,11 +2813,12 @@
       <c r="D15" t="s">
         <v>95</v>
       </c>
-      <c r="E15" s="2">
+      <c r="E15" s="3">
         <v>32539.68</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F15" s="3"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>2020</v>
       </c>
@@ -1765,11 +2831,12 @@
       <c r="D16" t="s">
         <v>97</v>
       </c>
-      <c r="E16" s="2">
+      <c r="E16" s="3">
         <v>30426.48</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F16" s="3"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>2020</v>
       </c>
@@ -1782,11 +2849,12 @@
       <c r="D17" t="s">
         <v>99</v>
       </c>
-      <c r="E17" s="2">
+      <c r="E17" s="3">
         <v>1993169.99</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F17" s="3"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>2020</v>
       </c>
@@ -1799,11 +2867,12 @@
       <c r="D18" t="s">
         <v>101</v>
       </c>
-      <c r="E18" s="2">
+      <c r="E18" s="3">
         <v>2550</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F18" s="3"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>2020</v>
       </c>
@@ -1816,11 +2885,12 @@
       <c r="D19" t="s">
         <v>65</v>
       </c>
-      <c r="E19" s="2">
+      <c r="E19" s="3">
         <v>175273.41</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F19" s="3"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>2020</v>
       </c>
@@ -1833,11 +2903,12 @@
       <c r="D20" t="s">
         <v>67</v>
       </c>
-      <c r="E20" s="2">
+      <c r="E20" s="3">
         <v>366410.64</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F20" s="3"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>2020</v>
       </c>
@@ -1850,11 +2921,12 @@
       <c r="D21" t="s">
         <v>71</v>
       </c>
-      <c r="E21" s="2">
+      <c r="E21" s="3">
         <v>43705.57</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F21" s="3"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>2020</v>
       </c>
@@ -1867,11 +2939,12 @@
       <c r="D22" t="s">
         <v>73</v>
       </c>
-      <c r="E22" s="2">
+      <c r="E22" s="3">
         <v>48404</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F22" s="3"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>2020</v>
       </c>
@@ -1884,11 +2957,12 @@
       <c r="D23" t="s">
         <v>103</v>
       </c>
-      <c r="E23">
+      <c r="E23" s="3">
         <v>294</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F23" s="3"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>2020</v>
       </c>
@@ -1901,11 +2975,12 @@
       <c r="D24" t="s">
         <v>105</v>
       </c>
-      <c r="E24">
+      <c r="E24" s="3">
         <v>437.18</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F24" s="3"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>2020</v>
       </c>
@@ -1918,8 +2993,18 @@
       <c r="D25" t="s">
         <v>85</v>
       </c>
-      <c r="E25" s="2">
+      <c r="E25" s="3">
         <v>218247.73</v>
+      </c>
+      <c r="F25" s="3"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E26" s="3">
+        <f>SUM(E2:E25)</f>
+        <v>3873657.0100000002</v>
+      </c>
+      <c r="F26" s="3">
+        <v>3873657.01</v>
       </c>
     </row>
   </sheetData>
@@ -1929,10 +3014,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{414A82B0-991A-4099-AE92-BF847839187E}">
-  <dimension ref="A1:E24"/>
+  <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:E1"/>
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1940,23 +3025,23 @@
     <col min="2" max="2" width="68.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.77734375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17.77734375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="14.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1973,7 +3058,7 @@
       <c r="D2" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="2">
+      <c r="E2" s="3">
         <v>52720.5</v>
       </c>
     </row>
@@ -1990,7 +3075,7 @@
       <c r="D3" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="2">
+      <c r="E3" s="3">
         <v>11882</v>
       </c>
     </row>
@@ -2007,7 +3092,7 @@
       <c r="D4" t="s">
         <v>107</v>
       </c>
-      <c r="E4" s="2">
+      <c r="E4" s="3">
         <v>55930</v>
       </c>
     </row>
@@ -2024,7 +3109,7 @@
       <c r="D5" t="s">
         <v>20</v>
       </c>
-      <c r="E5" s="2">
+      <c r="E5" s="3">
         <v>167968.45</v>
       </c>
     </row>
@@ -2041,7 +3126,7 @@
       <c r="D6" t="s">
         <v>87</v>
       </c>
-      <c r="E6" s="2">
+      <c r="E6" s="3">
         <v>335026.2</v>
       </c>
     </row>
@@ -2058,7 +3143,7 @@
       <c r="D7" t="s">
         <v>89</v>
       </c>
-      <c r="E7" s="2">
+      <c r="E7" s="3">
         <v>9885.66</v>
       </c>
     </row>
@@ -2075,7 +3160,7 @@
       <c r="D8" t="s">
         <v>91</v>
       </c>
-      <c r="E8" s="2">
+      <c r="E8" s="3">
         <v>15834</v>
       </c>
     </row>
@@ -2092,7 +3177,7 @@
       <c r="D9" t="s">
         <v>109</v>
       </c>
-      <c r="E9" s="2">
+      <c r="E9" s="3">
         <v>1708.8</v>
       </c>
     </row>
@@ -2109,7 +3194,7 @@
       <c r="D10" t="s">
         <v>111</v>
       </c>
-      <c r="E10" s="2">
+      <c r="E10" s="3">
         <v>50644</v>
       </c>
     </row>
@@ -2126,7 +3211,7 @@
       <c r="D11" t="s">
         <v>113</v>
       </c>
-      <c r="E11" s="2">
+      <c r="E11" s="3">
         <v>1209</v>
       </c>
     </row>
@@ -2143,7 +3228,7 @@
       <c r="D12" t="s">
         <v>41</v>
       </c>
-      <c r="E12">
+      <c r="E12" s="3">
         <v>480</v>
       </c>
     </row>
@@ -2160,7 +3245,7 @@
       <c r="D13" t="s">
         <v>45</v>
       </c>
-      <c r="E13" s="2">
+      <c r="E13" s="3">
         <v>263885.09999999998</v>
       </c>
     </row>
@@ -2177,7 +3262,7 @@
       <c r="D14" t="s">
         <v>115</v>
       </c>
-      <c r="E14">
+      <c r="E14" s="3">
         <v>251.96</v>
       </c>
     </row>
@@ -2194,7 +3279,7 @@
       <c r="D15" t="s">
         <v>53</v>
       </c>
-      <c r="E15" s="2">
+      <c r="E15" s="3">
         <v>20340</v>
       </c>
     </row>
@@ -2211,11 +3296,11 @@
       <c r="D16" t="s">
         <v>117</v>
       </c>
-      <c r="E16" s="2">
+      <c r="E16" s="3">
         <v>8835.6</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>2019</v>
       </c>
@@ -2228,11 +3313,11 @@
       <c r="D17" t="s">
         <v>97</v>
       </c>
-      <c r="E17">
+      <c r="E17" s="3">
         <v>934.2</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>2019</v>
       </c>
@@ -2245,11 +3330,11 @@
       <c r="D18" t="s">
         <v>99</v>
       </c>
-      <c r="E18" s="2">
+      <c r="E18" s="3">
         <v>2620174.8199999998</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>2019</v>
       </c>
@@ -2262,11 +3347,11 @@
       <c r="D19" t="s">
         <v>101</v>
       </c>
-      <c r="E19" s="2">
+      <c r="E19" s="3">
         <v>17985</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>2019</v>
       </c>
@@ -2279,11 +3364,11 @@
       <c r="D20" t="s">
         <v>65</v>
       </c>
-      <c r="E20" s="2">
+      <c r="E20" s="3">
         <v>14437.36</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>2019</v>
       </c>
@@ -2296,11 +3381,11 @@
       <c r="D21" t="s">
         <v>67</v>
       </c>
-      <c r="E21" s="2">
+      <c r="E21" s="3">
         <v>649019.98</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>2019</v>
       </c>
@@ -2313,11 +3398,11 @@
       <c r="D22" t="s">
         <v>71</v>
       </c>
-      <c r="E22" s="2">
+      <c r="E22" s="3">
         <v>6091.2</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>2019</v>
       </c>
@@ -2330,11 +3415,11 @@
       <c r="D23" t="s">
         <v>73</v>
       </c>
-      <c r="E23" s="2">
+      <c r="E23" s="3">
         <v>43008.4</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>2019</v>
       </c>
@@ -2347,8 +3432,17 @@
       <c r="D24" t="s">
         <v>119</v>
       </c>
-      <c r="E24" s="2">
+      <c r="E24" s="3">
         <v>5490.5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E25" s="3">
+        <f>SUM(E2:E24)</f>
+        <v>4353742.7300000004</v>
+      </c>
+      <c r="F25" s="3">
+        <v>4353742.7300000004</v>
       </c>
     </row>
   </sheetData>
@@ -2358,10 +3452,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0881AC5-6BED-47B2-A07C-310157D626D3}">
-  <dimension ref="A1:E31"/>
+  <dimension ref="A1:F32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2369,23 +3463,24 @@
     <col min="2" max="2" width="73.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.77734375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17.77734375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2402,7 +3497,7 @@
       <c r="D2" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="2">
+      <c r="E2" s="3">
         <v>38443.5</v>
       </c>
     </row>
@@ -2419,7 +3514,7 @@
       <c r="D3" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="2">
+      <c r="E3" s="3">
         <v>5950</v>
       </c>
     </row>
@@ -2436,7 +3531,7 @@
       <c r="D4" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="2">
+      <c r="E4" s="3">
         <v>3854</v>
       </c>
     </row>
@@ -2453,7 +3548,7 @@
       <c r="D5" t="s">
         <v>16</v>
       </c>
-      <c r="E5" s="2">
+      <c r="E5" s="3">
         <v>345674.49</v>
       </c>
     </row>
@@ -2470,7 +3565,7 @@
       <c r="D6" t="s">
         <v>20</v>
       </c>
-      <c r="E6" s="2">
+      <c r="E6" s="3">
         <v>5980.77</v>
       </c>
     </row>
@@ -2487,7 +3582,7 @@
       <c r="D7" t="s">
         <v>21</v>
       </c>
-      <c r="E7" s="2">
+      <c r="E7" s="3">
         <v>572936.11</v>
       </c>
     </row>
@@ -2504,7 +3599,7 @@
       <c r="D8" t="s">
         <v>23</v>
       </c>
-      <c r="E8" s="2">
+      <c r="E8" s="3">
         <v>2461</v>
       </c>
     </row>
@@ -2521,7 +3616,7 @@
       <c r="D9" t="s">
         <v>27</v>
       </c>
-      <c r="E9" s="2">
+      <c r="E9" s="3">
         <v>33434.99</v>
       </c>
     </row>
@@ -2538,7 +3633,7 @@
       <c r="D10" t="s">
         <v>35</v>
       </c>
-      <c r="E10" s="2">
+      <c r="E10" s="3">
         <v>595368</v>
       </c>
     </row>
@@ -2555,7 +3650,7 @@
       <c r="D11" t="s">
         <v>121</v>
       </c>
-      <c r="E11" s="2">
+      <c r="E11" s="3">
         <v>2239.17</v>
       </c>
     </row>
@@ -2572,7 +3667,7 @@
       <c r="D12" t="s">
         <v>89</v>
       </c>
-      <c r="E12" s="2">
+      <c r="E12" s="3">
         <v>5196</v>
       </c>
     </row>
@@ -2589,7 +3684,7 @@
       <c r="D13" t="s">
         <v>39</v>
       </c>
-      <c r="E13" s="2">
+      <c r="E13" s="3">
         <v>112531.4</v>
       </c>
     </row>
@@ -2606,7 +3701,7 @@
       <c r="D14" t="s">
         <v>91</v>
       </c>
-      <c r="E14" s="2">
+      <c r="E14" s="3">
         <v>8463</v>
       </c>
     </row>
@@ -2623,7 +3718,7 @@
       <c r="D15" t="s">
         <v>45</v>
       </c>
-      <c r="E15" s="2">
+      <c r="E15" s="3">
         <v>17322</v>
       </c>
     </row>
@@ -2640,11 +3735,11 @@
       <c r="D16" t="s">
         <v>49</v>
       </c>
-      <c r="E16" s="2">
+      <c r="E16" s="3">
         <v>45320.800000000003</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>2021</v>
       </c>
@@ -2657,11 +3752,11 @@
       <c r="D17" t="s">
         <v>97</v>
       </c>
-      <c r="E17" s="2">
+      <c r="E17" s="3">
         <v>4229.16</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>2021</v>
       </c>
@@ -2674,11 +3769,11 @@
       <c r="D18" t="s">
         <v>57</v>
       </c>
-      <c r="E18" s="2">
+      <c r="E18" s="3">
         <v>12711.84</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>2021</v>
       </c>
@@ -2691,11 +3786,11 @@
       <c r="D19" t="s">
         <v>59</v>
       </c>
-      <c r="E19" s="2">
+      <c r="E19" s="3">
         <v>8000.52</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>2021</v>
       </c>
@@ -2708,11 +3803,11 @@
       <c r="D20" t="s">
         <v>99</v>
       </c>
-      <c r="E20" s="2">
+      <c r="E20" s="3">
         <v>1372583.46</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>2021</v>
       </c>
@@ -2725,11 +3820,11 @@
       <c r="D21" t="s">
         <v>123</v>
       </c>
-      <c r="E21" s="2">
+      <c r="E21" s="3">
         <v>662688</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>2021</v>
       </c>
@@ -2742,11 +3837,11 @@
       <c r="D22" t="s">
         <v>65</v>
       </c>
-      <c r="E22" s="2">
+      <c r="E22" s="3">
         <v>181972.73</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>2021</v>
       </c>
@@ -2759,11 +3854,11 @@
       <c r="D23" t="s">
         <v>67</v>
       </c>
-      <c r="E23" s="2">
+      <c r="E23" s="3">
         <v>192416.77</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>2021</v>
       </c>
@@ -2776,11 +3871,11 @@
       <c r="D24" t="s">
         <v>69</v>
       </c>
-      <c r="E24" s="2">
+      <c r="E24" s="3">
         <v>82600</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>2021</v>
       </c>
@@ -2793,11 +3888,11 @@
       <c r="D25" t="s">
         <v>71</v>
       </c>
-      <c r="E25" s="2">
+      <c r="E25" s="3">
         <v>214692.57</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>2021</v>
       </c>
@@ -2810,11 +3905,11 @@
       <c r="D26" t="s">
         <v>73</v>
       </c>
-      <c r="E26" s="2">
+      <c r="E26" s="3">
         <v>12889.61</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>2021</v>
       </c>
@@ -2827,11 +3922,11 @@
       <c r="D27" t="s">
         <v>75</v>
       </c>
-      <c r="E27" s="2">
+      <c r="E27" s="3">
         <v>246562.46</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>2021</v>
       </c>
@@ -2844,11 +3939,11 @@
       <c r="D28" t="s">
         <v>77</v>
       </c>
-      <c r="E28" s="2">
+      <c r="E28" s="3">
         <v>11449.12</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>2021</v>
       </c>
@@ -2861,11 +3956,11 @@
       <c r="D29" t="s">
         <v>81</v>
       </c>
-      <c r="E29" s="2">
+      <c r="E29" s="3">
         <v>1696.97</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>2021</v>
       </c>
@@ -2878,11 +3973,11 @@
       <c r="D30" t="s">
         <v>105</v>
       </c>
-      <c r="E30">
+      <c r="E30" s="3">
         <v>766</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>2021</v>
       </c>
@@ -2895,11 +3990,81 @@
       <c r="D31" t="s">
         <v>85</v>
       </c>
-      <c r="E31" s="2">
+      <c r="E31" s="3">
         <v>269571.93</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E32" s="3">
+        <f>SUM(E2:E31)</f>
+        <v>5070006.37</v>
+      </c>
+      <c r="F32" s="4">
+        <v>5070006.37</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{300D45A2-0669-4D2F-9E92-E8A9D47BFFF4}">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="94" workbookViewId="0">
+      <selection activeCell="Q8" sqref="Q8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="15.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2019</v>
+      </c>
+      <c r="B3" s="3">
+        <v>4353742.7300000004</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>2020</v>
+      </c>
+      <c r="B4" s="3">
+        <v>3873657.01</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>2021</v>
+      </c>
+      <c r="B5" s="4">
+        <v>5070006.37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>2022</v>
+      </c>
+      <c r="B6" s="5">
+        <v>4593269.88</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>